<commit_message>
Finished workig on generate_payment_gst_sum and generate_product_gst_sum. Have started working on generate_detail_sales_reg
</commit_message>
<xml_diff>
--- a/detail_sales_sum_df.xlsx
+++ b/detail_sales_sum_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>NET QTY</t>
   </si>
@@ -40,10 +40,76 @@
     <t>GST RATE</t>
   </si>
   <si>
+    <t>GrossAmt-BillAmt</t>
+  </si>
+  <si>
+    <t>ADDITION CHRGS GST 03%</t>
+  </si>
+  <si>
+    <t>SALES DISCOUNT GST 03%</t>
+  </si>
+  <si>
+    <t>FLAT DISCOUNT GST 03%</t>
+  </si>
+  <si>
+    <t>LESS EXCHANGE GST 03%</t>
+  </si>
+  <si>
+    <t>ADDITION CHRGS GST 05%</t>
+  </si>
+  <si>
+    <t>SALES DISCOUNT GST 05%</t>
+  </si>
+  <si>
+    <t>FLAT DISCOUNT GST 05%</t>
+  </si>
+  <si>
+    <t>LESS EXCHANGE GST 05%</t>
+  </si>
+  <si>
+    <t>ADDITION CHRGS GST 12%</t>
+  </si>
+  <si>
+    <t>SALES DISCOUNT GST 12%</t>
+  </si>
+  <si>
+    <t>FLAT DISCOUNT GST 12%</t>
+  </si>
+  <si>
+    <t>LESS EXCHANGE GST 12%</t>
+  </si>
+  <si>
+    <t>ADDITION CHRGS GST 18%</t>
+  </si>
+  <si>
+    <t>SALES DISCOUNT GST 18%</t>
+  </si>
+  <si>
+    <t>FLAT DISCOUNT GST 18%</t>
+  </si>
+  <si>
+    <t>LESS EXCHANGE GST 18%</t>
+  </si>
+  <si>
+    <t>ADDITION CHRGS GST WISE</t>
+  </si>
+  <si>
+    <t>SALES DISCOUNT GST WISE</t>
+  </si>
+  <si>
+    <t>FLAT DISCOUNT GST WISE</t>
+  </si>
+  <si>
+    <t>LESS EXCHANGE GST WISE</t>
+  </si>
+  <si>
     <t>GST TAX</t>
   </si>
   <si>
     <t>GROSS SALES</t>
+  </si>
+  <si>
+    <t>GROSS MRP</t>
   </si>
   <si>
     <t>NET SALES</t>
@@ -407,13 +473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:AI98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +516,74 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -468,19 +600,25 @@
         <v>12</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>-182.04</v>
       </c>
-      <c r="K2">
+      <c r="AF2">
         <v>-1699</v>
       </c>
-      <c r="L2">
+      <c r="AG2">
+        <v>-1699</v>
+      </c>
+      <c r="AH2">
         <v>-1516.96</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="AI2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,19 +635,25 @@
         <v>12</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
         <v>-192.75</v>
       </c>
-      <c r="K3">
+      <c r="AF3">
         <v>-1799</v>
       </c>
-      <c r="L3">
+      <c r="AG3">
+        <v>-1799</v>
+      </c>
+      <c r="AH3">
         <v>-1606.25</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="AI3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -526,19 +670,25 @@
         <v>12</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
         <v>160.61</v>
       </c>
-      <c r="K4">
+      <c r="AF4">
         <v>1499</v>
       </c>
-      <c r="L4">
+      <c r="AG4">
+        <v>1499</v>
+      </c>
+      <c r="AH4">
         <v>1338.39</v>
       </c>
-      <c r="M4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="AI4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -558,42 +708,75 @@
         <v>5</v>
       </c>
       <c r="J5">
+        <v>708</v>
+      </c>
+      <c r="Q5">
+        <v>-144.31</v>
+      </c>
+      <c r="AC5">
+        <v>-144.31</v>
+      </c>
+      <c r="AE5">
         <v>95.41</v>
       </c>
-      <c r="K5">
+      <c r="AF5">
         <v>2003.68</v>
       </c>
-      <c r="L5">
+      <c r="AG5">
+        <v>2147.99</v>
+      </c>
+      <c r="AH5">
         <v>1908.27</v>
       </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="AI5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
+      <c r="C6">
+        <v>10538</v>
+      </c>
+      <c r="F6">
+        <v>-708</v>
+      </c>
+      <c r="H6">
+        <v>9830</v>
+      </c>
       <c r="I6">
         <v>12</v>
       </c>
       <c r="J6">
+        <v>708</v>
+      </c>
+      <c r="U6">
+        <v>-563.6900000000001</v>
+      </c>
+      <c r="AC6">
+        <v>-563.6900000000001</v>
+      </c>
+      <c r="AE6">
         <v>838.53</v>
       </c>
-      <c r="K6">
+      <c r="AF6">
         <v>7826.32</v>
       </c>
-      <c r="L6">
+      <c r="AG6">
+        <v>8390.01</v>
+      </c>
+      <c r="AH6">
         <v>6987.79</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="AI6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -610,19 +793,25 @@
         <v>12</v>
       </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
         <v>465</v>
       </c>
-      <c r="K7">
+      <c r="AF7">
         <v>4340</v>
       </c>
-      <c r="L7">
+      <c r="AG7">
+        <v>4340</v>
+      </c>
+      <c r="AH7">
         <v>3875</v>
       </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="AI7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -639,19 +828,25 @@
         <v>12</v>
       </c>
       <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
         <v>1145.14</v>
       </c>
-      <c r="K8">
+      <c r="AF8">
         <v>10688</v>
       </c>
-      <c r="L8">
+      <c r="AG8">
+        <v>10688</v>
+      </c>
+      <c r="AH8">
         <v>9542.860000000001</v>
       </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="AI8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -668,19 +863,25 @@
         <v>12</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
         <v>165.96</v>
       </c>
-      <c r="K9">
+      <c r="AF9">
         <v>1549</v>
       </c>
-      <c r="L9">
+      <c r="AG9">
+        <v>1549</v>
+      </c>
+      <c r="AH9">
         <v>1383.04</v>
       </c>
-      <c r="M9">
+      <c r="AI9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -697,19 +898,25 @@
         <v>5</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
         <v>85.23999999999999</v>
       </c>
-      <c r="K10">
+      <c r="AF10">
         <v>1790</v>
       </c>
-      <c r="L10">
+      <c r="AG10">
+        <v>1790</v>
+      </c>
+      <c r="AH10">
         <v>1704.76</v>
       </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="AI10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -726,19 +933,25 @@
         <v>12</v>
       </c>
       <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
         <v>481.39</v>
       </c>
-      <c r="K11">
+      <c r="AF11">
         <v>4493</v>
       </c>
-      <c r="L11">
+      <c r="AG11">
+        <v>4493</v>
+      </c>
+      <c r="AH11">
         <v>4011.61</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="AI11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -755,42 +968,60 @@
         <v>5</v>
       </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
         <v>47.57</v>
       </c>
-      <c r="K12">
+      <c r="AF12">
         <v>999</v>
       </c>
-      <c r="L12">
+      <c r="AG12">
+        <v>999</v>
+      </c>
+      <c r="AH12">
         <v>951.4299999999999</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="AI12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="C13">
+        <v>3697</v>
+      </c>
+      <c r="H13">
+        <v>3697</v>
+      </c>
       <c r="I13">
         <v>12</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <v>289.07</v>
       </c>
-      <c r="K13">
+      <c r="AF13">
         <v>2698</v>
       </c>
-      <c r="L13">
+      <c r="AG13">
+        <v>2698</v>
+      </c>
+      <c r="AH13">
         <v>2408.93</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="AI13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -810,19 +1041,31 @@
         <v>5</v>
       </c>
       <c r="J14">
+        <v>1695</v>
+      </c>
+      <c r="Q14">
+        <v>-1695</v>
+      </c>
+      <c r="AC14">
+        <v>-1695</v>
+      </c>
+      <c r="AE14">
         <v>4.19</v>
       </c>
-      <c r="K14">
+      <c r="AF14">
         <v>88</v>
       </c>
-      <c r="L14">
+      <c r="AG14">
+        <v>1783</v>
+      </c>
+      <c r="AH14">
         <v>83.81</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="AI14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -842,19 +1085,31 @@
         <v>12</v>
       </c>
       <c r="J15">
+        <v>228</v>
+      </c>
+      <c r="V15">
+        <v>-228</v>
+      </c>
+      <c r="AD15">
+        <v>-228</v>
+      </c>
+      <c r="AE15">
         <v>328.07</v>
       </c>
-      <c r="K15">
+      <c r="AF15">
         <v>3062</v>
       </c>
-      <c r="L15">
+      <c r="AG15">
+        <v>3290</v>
+      </c>
+      <c r="AH15">
         <v>2733.93</v>
       </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="AI15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -874,19 +1129,31 @@
         <v>12</v>
       </c>
       <c r="J16">
+        <v>137</v>
+      </c>
+      <c r="V16">
+        <v>-137</v>
+      </c>
+      <c r="AD16">
+        <v>-137</v>
+      </c>
+      <c r="AE16">
         <v>156.21</v>
       </c>
-      <c r="K16">
+      <c r="AF16">
         <v>1458</v>
       </c>
-      <c r="L16">
+      <c r="AG16">
+        <v>1595</v>
+      </c>
+      <c r="AH16">
         <v>1301.79</v>
       </c>
-      <c r="M16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="AI16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -903,19 +1170,25 @@
         <v>12</v>
       </c>
       <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
         <v>566.6799999999999</v>
       </c>
-      <c r="K17">
+      <c r="AF17">
         <v>5289</v>
       </c>
-      <c r="L17">
+      <c r="AG17">
+        <v>5289</v>
+      </c>
+      <c r="AH17">
         <v>4722.32</v>
       </c>
-      <c r="M17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="AI17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -932,19 +1205,25 @@
         <v>3</v>
       </c>
       <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
         <v>5.83</v>
       </c>
-      <c r="K18">
+      <c r="AF18">
         <v>200</v>
       </c>
-      <c r="L18">
+      <c r="AG18">
+        <v>200</v>
+      </c>
+      <c r="AH18">
         <v>194.17</v>
       </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="AI18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -964,42 +1243,75 @@
         <v>5</v>
       </c>
       <c r="J19">
+        <v>769</v>
+      </c>
+      <c r="P19">
+        <v>-119.5</v>
+      </c>
+      <c r="AB19">
+        <v>-119.5</v>
+      </c>
+      <c r="AE19">
         <v>51.21</v>
       </c>
-      <c r="K19">
+      <c r="AF19">
         <v>1075.5</v>
       </c>
-      <c r="L19">
+      <c r="AG19">
+        <v>1195</v>
+      </c>
+      <c r="AH19">
         <v>1024.29</v>
       </c>
-      <c r="M19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="AI19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
+      <c r="C20">
+        <v>7690</v>
+      </c>
+      <c r="E20">
+        <v>-769</v>
+      </c>
+      <c r="H20">
+        <v>6921</v>
+      </c>
       <c r="I20">
         <v>12</v>
       </c>
       <c r="J20">
+        <v>769</v>
+      </c>
+      <c r="T20">
+        <v>-649.5</v>
+      </c>
+      <c r="AB20">
+        <v>-649.5</v>
+      </c>
+      <c r="AE20">
         <v>626.3</v>
       </c>
-      <c r="K20">
+      <c r="AF20">
         <v>5845.5</v>
       </c>
-      <c r="L20">
+      <c r="AG20">
+        <v>6495</v>
+      </c>
+      <c r="AH20">
         <v>5219.2</v>
       </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="AI20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1016,19 +1328,25 @@
         <v>12</v>
       </c>
       <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
         <v>326.14</v>
       </c>
-      <c r="K21">
+      <c r="AF21">
         <v>3044</v>
       </c>
-      <c r="L21">
+      <c r="AG21">
+        <v>3044</v>
+      </c>
+      <c r="AH21">
         <v>2717.86</v>
       </c>
-      <c r="M21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="AI21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1045,19 +1363,25 @@
         <v>12</v>
       </c>
       <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
         <v>374.79</v>
       </c>
-      <c r="K22">
+      <c r="AF22">
         <v>3498</v>
       </c>
-      <c r="L22">
+      <c r="AG22">
+        <v>3498</v>
+      </c>
+      <c r="AH22">
         <v>3123.21</v>
       </c>
-      <c r="M22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="AI22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1074,19 +1398,25 @@
         <v>12</v>
       </c>
       <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
         <v>748.29</v>
       </c>
-      <c r="K23">
+      <c r="AF23">
         <v>6984</v>
       </c>
-      <c r="L23">
+      <c r="AG23">
+        <v>6984</v>
+      </c>
+      <c r="AH23">
         <v>6235.71</v>
       </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="AI23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1106,19 +1436,31 @@
         <v>12</v>
       </c>
       <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="V24">
+        <v>-50</v>
+      </c>
+      <c r="AD24">
+        <v>-50</v>
+      </c>
+      <c r="AE24">
         <v>294</v>
       </c>
-      <c r="K24">
+      <c r="AF24">
         <v>2744</v>
       </c>
-      <c r="L24">
+      <c r="AG24">
+        <v>2794</v>
+      </c>
+      <c r="AH24">
         <v>2450</v>
       </c>
-      <c r="M24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="AI24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1138,19 +1480,31 @@
         <v>5</v>
       </c>
       <c r="J25">
+        <v>45</v>
+      </c>
+      <c r="R25">
+        <v>-45</v>
+      </c>
+      <c r="AD25">
+        <v>-45</v>
+      </c>
+      <c r="AE25">
         <v>47.62</v>
       </c>
-      <c r="K25">
+      <c r="AF25">
         <v>1000</v>
       </c>
-      <c r="L25">
+      <c r="AG25">
+        <v>1045</v>
+      </c>
+      <c r="AH25">
         <v>952.38</v>
       </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="AI25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1167,19 +1521,25 @@
         <v>5</v>
       </c>
       <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
         <v>120.48</v>
       </c>
-      <c r="K26">
+      <c r="AF26">
         <v>2530</v>
       </c>
-      <c r="L26">
+      <c r="AG26">
+        <v>2530</v>
+      </c>
+      <c r="AH26">
         <v>2409.52</v>
       </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="AI26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1196,19 +1556,25 @@
         <v>12</v>
       </c>
       <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
         <v>1028.14</v>
       </c>
-      <c r="K27">
+      <c r="AF27">
         <v>9596</v>
       </c>
-      <c r="L27">
+      <c r="AG27">
+        <v>9596</v>
+      </c>
+      <c r="AH27">
         <v>8567.860000000001</v>
       </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="AI27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1228,19 +1594,31 @@
         <v>12</v>
       </c>
       <c r="J28">
+        <v>-500</v>
+      </c>
+      <c r="S28">
+        <v>500</v>
+      </c>
+      <c r="AA28">
+        <v>500</v>
+      </c>
+      <c r="AE28">
         <v>482.14</v>
       </c>
-      <c r="K28">
+      <c r="AF28">
         <v>4500</v>
       </c>
-      <c r="L28">
+      <c r="AG28">
+        <v>4000</v>
+      </c>
+      <c r="AH28">
         <v>4017.86</v>
       </c>
-      <c r="M28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="AI28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1257,19 +1635,25 @@
         <v>12</v>
       </c>
       <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
         <v>438.11</v>
       </c>
-      <c r="K29">
+      <c r="AF29">
         <v>4089</v>
       </c>
-      <c r="L29">
+      <c r="AG29">
+        <v>4089</v>
+      </c>
+      <c r="AH29">
         <v>3650.89</v>
       </c>
-      <c r="M29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="AI29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1286,19 +1670,25 @@
         <v>5</v>
       </c>
       <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
         <v>47.38</v>
       </c>
-      <c r="K30">
+      <c r="AF30">
         <v>995</v>
       </c>
-      <c r="L30">
+      <c r="AG30">
+        <v>995</v>
+      </c>
+      <c r="AH30">
         <v>947.62</v>
       </c>
-      <c r="M30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="AI30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1315,19 +1705,25 @@
         <v>12</v>
       </c>
       <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
         <v>331.61</v>
       </c>
-      <c r="K31">
+      <c r="AF31">
         <v>3095</v>
       </c>
-      <c r="L31">
+      <c r="AG31">
+        <v>3095</v>
+      </c>
+      <c r="AH31">
         <v>2763.39</v>
       </c>
-      <c r="M31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="AI31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1344,19 +1740,25 @@
         <v>5</v>
       </c>
       <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
         <v>49.76</v>
       </c>
-      <c r="K32">
+      <c r="AF32">
         <v>1045</v>
       </c>
-      <c r="L32">
+      <c r="AG32">
+        <v>1045</v>
+      </c>
+      <c r="AH32">
         <v>995.24</v>
       </c>
-      <c r="M32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="AI32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1373,19 +1775,25 @@
         <v>12</v>
       </c>
       <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
         <v>1166.79</v>
       </c>
-      <c r="K33">
+      <c r="AF33">
         <v>10890</v>
       </c>
-      <c r="L33">
+      <c r="AG33">
+        <v>10890</v>
+      </c>
+      <c r="AH33">
         <v>9723.209999999999</v>
       </c>
-      <c r="M33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="AI33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1405,42 +1813,75 @@
         <v>5</v>
       </c>
       <c r="J34">
+        <v>201</v>
+      </c>
+      <c r="R34">
+        <v>-126.29</v>
+      </c>
+      <c r="AD34">
+        <v>-126.29</v>
+      </c>
+      <c r="AE34">
         <v>90.18000000000001</v>
       </c>
-      <c r="K34">
+      <c r="AF34">
         <v>1893.71</v>
       </c>
-      <c r="L34">
+      <c r="AG34">
+        <v>2020</v>
+      </c>
+      <c r="AH34">
         <v>1803.53</v>
       </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="AI34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
+      <c r="C35">
+        <v>3215</v>
+      </c>
+      <c r="G35">
+        <v>-201</v>
+      </c>
+      <c r="H35">
+        <v>3014</v>
+      </c>
       <c r="I35">
         <v>12</v>
       </c>
       <c r="J35">
+        <v>201</v>
+      </c>
+      <c r="V35">
+        <v>-74.70999999999999</v>
+      </c>
+      <c r="AD35">
+        <v>-74.70999999999999</v>
+      </c>
+      <c r="AE35">
         <v>120.03</v>
       </c>
-      <c r="K35">
+      <c r="AF35">
         <v>1120.29</v>
       </c>
-      <c r="L35">
+      <c r="AG35">
+        <v>1195</v>
+      </c>
+      <c r="AH35">
         <v>1000.26</v>
       </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="AI35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1460,42 +1901,75 @@
         <v>5</v>
       </c>
       <c r="J36">
+        <v>340</v>
+      </c>
+      <c r="R36">
+        <v>-119.85</v>
+      </c>
+      <c r="AD36">
+        <v>-119.85</v>
+      </c>
+      <c r="AE36">
         <v>51.2</v>
       </c>
-      <c r="K36">
+      <c r="AF36">
         <v>1075.15</v>
       </c>
-      <c r="L36">
+      <c r="AG36">
+        <v>1195</v>
+      </c>
+      <c r="AH36">
         <v>1023.95</v>
       </c>
-      <c r="M36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="AI36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
+      <c r="C37">
+        <v>3390</v>
+      </c>
+      <c r="G37">
+        <v>-340</v>
+      </c>
+      <c r="H37">
+        <v>3050</v>
+      </c>
       <c r="I37">
         <v>12</v>
       </c>
       <c r="J37">
+        <v>340</v>
+      </c>
+      <c r="V37">
+        <v>-220.15</v>
+      </c>
+      <c r="AD37">
+        <v>-220.15</v>
+      </c>
+      <c r="AE37">
         <v>211.59</v>
       </c>
-      <c r="K37">
+      <c r="AF37">
         <v>1974.85</v>
       </c>
-      <c r="L37">
+      <c r="AG37">
+        <v>2195</v>
+      </c>
+      <c r="AH37">
         <v>1763.26</v>
       </c>
-      <c r="M37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="AI37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1512,19 +1986,25 @@
         <v>12</v>
       </c>
       <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
         <v>203.04</v>
       </c>
-      <c r="K38">
+      <c r="AF38">
         <v>1895</v>
       </c>
-      <c r="L38">
+      <c r="AG38">
+        <v>1895</v>
+      </c>
+      <c r="AH38">
         <v>1691.96</v>
       </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="AI38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1541,19 +2021,25 @@
         <v>12</v>
       </c>
       <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="AE39">
         <v>438.75</v>
       </c>
-      <c r="K39">
+      <c r="AF39">
         <v>4095</v>
       </c>
-      <c r="L39">
+      <c r="AG39">
+        <v>4095</v>
+      </c>
+      <c r="AH39">
         <v>3656.25</v>
       </c>
-      <c r="M39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="AI39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1573,42 +2059,75 @@
         <v>5</v>
       </c>
       <c r="J40">
+        <v>657</v>
+      </c>
+      <c r="R40">
+        <v>-132.04</v>
+      </c>
+      <c r="AD40">
+        <v>-132.04</v>
+      </c>
+      <c r="AE40">
         <v>188</v>
       </c>
-      <c r="K40">
+      <c r="AF40">
         <v>3947.96</v>
       </c>
-      <c r="L40">
+      <c r="AG40">
+        <v>4080</v>
+      </c>
+      <c r="AH40">
         <v>3759.96</v>
       </c>
-      <c r="M40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="AI40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
         <v>9</v>
       </c>
+      <c r="C41">
+        <v>20301</v>
+      </c>
+      <c r="G41">
+        <v>-657</v>
+      </c>
+      <c r="H41">
+        <v>19644</v>
+      </c>
       <c r="I41">
         <v>12</v>
       </c>
       <c r="J41">
+        <v>657</v>
+      </c>
+      <c r="V41">
+        <v>-524.96</v>
+      </c>
+      <c r="AD41">
+        <v>-524.96</v>
+      </c>
+      <c r="AE41">
         <v>1681.72</v>
       </c>
-      <c r="K41">
+      <c r="AF41">
         <v>15696.04</v>
       </c>
-      <c r="L41">
+      <c r="AG41">
+        <v>16221</v>
+      </c>
+      <c r="AH41">
         <v>14014.32</v>
       </c>
-      <c r="M41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="AI41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1628,19 +2147,31 @@
         <v>12</v>
       </c>
       <c r="J42">
+        <v>299</v>
+      </c>
+      <c r="T42">
+        <v>-299</v>
+      </c>
+      <c r="AB42">
+        <v>-299</v>
+      </c>
+      <c r="AE42">
         <v>288.32</v>
       </c>
-      <c r="K42">
+      <c r="AF42">
         <v>2691</v>
       </c>
-      <c r="L42">
+      <c r="AG42">
+        <v>2990</v>
+      </c>
+      <c r="AH42">
         <v>2402.68</v>
       </c>
-      <c r="M42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="AI42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1657,19 +2188,25 @@
         <v>5</v>
       </c>
       <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="AE43">
         <v>139.76</v>
       </c>
-      <c r="K43">
+      <c r="AF43">
         <v>2935</v>
       </c>
-      <c r="L43">
+      <c r="AG43">
+        <v>2935</v>
+      </c>
+      <c r="AH43">
         <v>2795.24</v>
       </c>
-      <c r="M43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="AI43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1689,42 +2226,75 @@
         <v>5</v>
       </c>
       <c r="J44">
+        <v>841</v>
+      </c>
+      <c r="R44">
+        <v>-405.39</v>
+      </c>
+      <c r="AD44">
+        <v>-405.39</v>
+      </c>
+      <c r="AE44">
         <v>47.12</v>
       </c>
-      <c r="K44">
+      <c r="AF44">
         <v>989.61</v>
       </c>
-      <c r="L44">
+      <c r="AG44">
+        <v>1395</v>
+      </c>
+      <c r="AH44">
         <v>942.49</v>
       </c>
-      <c r="M44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="AI44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
+      <c r="C45">
+        <v>2894</v>
+      </c>
+      <c r="G45">
+        <v>-841</v>
+      </c>
+      <c r="H45">
+        <v>2053</v>
+      </c>
       <c r="I45">
         <v>12</v>
       </c>
       <c r="J45">
+        <v>841</v>
+      </c>
+      <c r="V45">
+        <v>-435.61</v>
+      </c>
+      <c r="AD45">
+        <v>-435.61</v>
+      </c>
+      <c r="AE45">
         <v>113.93</v>
       </c>
-      <c r="K45">
+      <c r="AF45">
         <v>1063.39</v>
       </c>
-      <c r="L45">
+      <c r="AG45">
+        <v>1499</v>
+      </c>
+      <c r="AH45">
         <v>949.46</v>
       </c>
-      <c r="M45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="AI45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1741,19 +2311,25 @@
         <v>12</v>
       </c>
       <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="AE46">
         <v>459.11</v>
       </c>
-      <c r="K46">
+      <c r="AF46">
         <v>4285</v>
       </c>
-      <c r="L46">
+      <c r="AG46">
+        <v>4285</v>
+      </c>
+      <c r="AH46">
         <v>3825.89</v>
       </c>
-      <c r="M46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="AI46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1770,19 +2346,25 @@
         <v>12</v>
       </c>
       <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="AE47">
         <v>481.07</v>
       </c>
-      <c r="K47">
+      <c r="AF47">
         <v>4490</v>
       </c>
-      <c r="L47">
+      <c r="AG47">
+        <v>4490</v>
+      </c>
+      <c r="AH47">
         <v>4008.93</v>
       </c>
-      <c r="M47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="AI47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1802,19 +2384,31 @@
         <v>12</v>
       </c>
       <c r="J48">
+        <v>-100</v>
+      </c>
+      <c r="S48">
+        <v>100</v>
+      </c>
+      <c r="AA48">
+        <v>100</v>
+      </c>
+      <c r="AE48">
         <v>471.21</v>
       </c>
-      <c r="K48">
+      <c r="AF48">
         <v>4398</v>
       </c>
-      <c r="L48">
+      <c r="AG48">
+        <v>4298</v>
+      </c>
+      <c r="AH48">
         <v>3926.79</v>
       </c>
-      <c r="M48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="AI48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1831,19 +2425,25 @@
         <v>12</v>
       </c>
       <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="AE49">
         <v>149.46</v>
       </c>
-      <c r="K49">
+      <c r="AF49">
         <v>1395</v>
       </c>
-      <c r="L49">
+      <c r="AG49">
+        <v>1395</v>
+      </c>
+      <c r="AH49">
         <v>1245.54</v>
       </c>
-      <c r="M49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="AI49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1863,42 +2463,75 @@
         <v>5</v>
       </c>
       <c r="J50">
+        <v>395</v>
+      </c>
+      <c r="R50">
+        <v>-160.79</v>
+      </c>
+      <c r="AD50">
+        <v>-160.79</v>
+      </c>
+      <c r="AE50">
         <v>44.49</v>
       </c>
-      <c r="K50">
+      <c r="AF50">
         <v>934.21</v>
       </c>
-      <c r="L50">
+      <c r="AG50">
+        <v>1095</v>
+      </c>
+      <c r="AH50">
         <v>889.72</v>
       </c>
-      <c r="M50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="AI50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
+      <c r="C51">
+        <v>2690</v>
+      </c>
+      <c r="G51">
+        <v>-395</v>
+      </c>
+      <c r="H51">
+        <v>2295</v>
+      </c>
       <c r="I51">
         <v>12</v>
       </c>
       <c r="J51">
+        <v>395</v>
+      </c>
+      <c r="V51">
+        <v>-234.21</v>
+      </c>
+      <c r="AD51">
+        <v>-234.21</v>
+      </c>
+      <c r="AE51">
         <v>145.8</v>
       </c>
-      <c r="K51">
+      <c r="AF51">
         <v>1360.79</v>
       </c>
-      <c r="L51">
+      <c r="AG51">
+        <v>1595</v>
+      </c>
+      <c r="AH51">
         <v>1214.99</v>
       </c>
-      <c r="M51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="AI51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1915,19 +2548,25 @@
         <v>12</v>
       </c>
       <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
         <v>170.89</v>
       </c>
-      <c r="K52">
+      <c r="AF52">
         <v>1595</v>
       </c>
-      <c r="L52">
+      <c r="AG52">
+        <v>1595</v>
+      </c>
+      <c r="AH52">
         <v>1424.11</v>
       </c>
-      <c r="M52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="AI52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1944,19 +2583,25 @@
         <v>12</v>
       </c>
       <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="AE53">
         <v>470.79</v>
       </c>
-      <c r="K53">
+      <c r="AF53">
         <v>4394</v>
       </c>
-      <c r="L53">
+      <c r="AG53">
+        <v>4394</v>
+      </c>
+      <c r="AH53">
         <v>3923.21</v>
       </c>
-      <c r="M53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="AI53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1973,19 +2618,25 @@
         <v>12</v>
       </c>
       <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
         <v>342.21</v>
       </c>
-      <c r="K54">
+      <c r="AF54">
         <v>3194</v>
       </c>
-      <c r="L54">
+      <c r="AG54">
+        <v>3194</v>
+      </c>
+      <c r="AH54">
         <v>2851.79</v>
       </c>
-      <c r="M54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="AI54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2002,19 +2653,25 @@
         <v>12</v>
       </c>
       <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="AE55">
         <v>801.86</v>
       </c>
-      <c r="K55">
+      <c r="AF55">
         <v>7484</v>
       </c>
-      <c r="L55">
+      <c r="AG55">
+        <v>7484</v>
+      </c>
+      <c r="AH55">
         <v>6682.14</v>
       </c>
-      <c r="M55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="AI55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2034,19 +2691,31 @@
         <v>12</v>
       </c>
       <c r="J56">
+        <v>299</v>
+      </c>
+      <c r="T56">
+        <v>-299.5</v>
+      </c>
+      <c r="AB56">
+        <v>-299.5</v>
+      </c>
+      <c r="AE56">
         <v>288.86</v>
       </c>
-      <c r="K56">
+      <c r="AF56">
         <v>2696</v>
       </c>
-      <c r="L56">
+      <c r="AG56">
+        <v>2995</v>
+      </c>
+      <c r="AH56">
         <v>2407.14</v>
       </c>
-      <c r="M56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="AI56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2063,19 +2732,25 @@
         <v>5</v>
       </c>
       <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="AE57">
         <v>142.14</v>
       </c>
-      <c r="K57">
+      <c r="AF57">
         <v>2985</v>
       </c>
-      <c r="L57">
+      <c r="AG57">
+        <v>2985</v>
+      </c>
+      <c r="AH57">
         <v>2842.86</v>
       </c>
-      <c r="M57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="AI57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2092,19 +2767,25 @@
         <v>12</v>
       </c>
       <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="AE58">
         <v>491.79</v>
       </c>
-      <c r="K58">
+      <c r="AF58">
         <v>4590</v>
       </c>
-      <c r="L58">
+      <c r="AG58">
+        <v>4590</v>
+      </c>
+      <c r="AH58">
         <v>4098.21</v>
       </c>
-      <c r="M58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="AI58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2121,19 +2802,25 @@
         <v>12</v>
       </c>
       <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="AE59">
         <v>299.36</v>
       </c>
-      <c r="K59">
+      <c r="AF59">
         <v>2794</v>
       </c>
-      <c r="L59">
+      <c r="AG59">
+        <v>2794</v>
+      </c>
+      <c r="AH59">
         <v>2494.64</v>
       </c>
-      <c r="M59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="AI59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2150,19 +2837,25 @@
         <v>12</v>
       </c>
       <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="AE60">
         <v>224.89</v>
       </c>
-      <c r="K60">
+      <c r="AF60">
         <v>2099</v>
       </c>
-      <c r="L60">
+      <c r="AG60">
+        <v>2099</v>
+      </c>
+      <c r="AH60">
         <v>1874.11</v>
       </c>
-      <c r="M60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="AI60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2182,19 +2875,31 @@
         <v>12</v>
       </c>
       <c r="J61">
+        <v>137</v>
+      </c>
+      <c r="V61">
+        <v>-137</v>
+      </c>
+      <c r="AD61">
+        <v>-137</v>
+      </c>
+      <c r="AE61">
         <v>613.0700000000001</v>
       </c>
-      <c r="K61">
+      <c r="AF61">
         <v>5722</v>
       </c>
-      <c r="L61">
+      <c r="AG61">
+        <v>5859</v>
+      </c>
+      <c r="AH61">
         <v>5108.93</v>
       </c>
-      <c r="M61">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="AI61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2211,19 +2916,25 @@
         <v>5</v>
       </c>
       <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="AE62">
         <v>25.67</v>
       </c>
-      <c r="K62">
+      <c r="AF62">
         <v>539</v>
       </c>
-      <c r="L62">
+      <c r="AG62">
+        <v>539</v>
+      </c>
+      <c r="AH62">
         <v>513.33</v>
       </c>
-      <c r="M62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="AI62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2240,19 +2951,25 @@
         <v>12</v>
       </c>
       <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="AE63">
         <v>353.04</v>
       </c>
-      <c r="K63">
+      <c r="AF63">
         <v>3295</v>
       </c>
-      <c r="L63">
+      <c r="AG63">
+        <v>3295</v>
+      </c>
+      <c r="AH63">
         <v>2941.96</v>
       </c>
-      <c r="M63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="AI63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2269,19 +2986,25 @@
         <v>5</v>
       </c>
       <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="AE64">
         <v>97.14</v>
       </c>
-      <c r="K64">
+      <c r="AF64">
         <v>2040</v>
       </c>
-      <c r="L64">
+      <c r="AG64">
+        <v>2040</v>
+      </c>
+      <c r="AH64">
         <v>1942.86</v>
       </c>
-      <c r="M64">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="AI64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2298,42 +3021,60 @@
         <v>5</v>
       </c>
       <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="AE65">
         <v>47.38</v>
       </c>
-      <c r="K65">
+      <c r="AF65">
         <v>995</v>
       </c>
-      <c r="L65">
+      <c r="AG65">
+        <v>995</v>
+      </c>
+      <c r="AH65">
         <v>947.62</v>
       </c>
-      <c r="M65">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="AI65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
+      <c r="C66">
+        <v>4985</v>
+      </c>
+      <c r="H66">
+        <v>4985</v>
+      </c>
       <c r="I66">
         <v>12</v>
       </c>
       <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="AE66">
         <v>427.5</v>
       </c>
-      <c r="K66">
+      <c r="AF66">
         <v>3990</v>
       </c>
-      <c r="L66">
+      <c r="AG66">
+        <v>3990</v>
+      </c>
+      <c r="AH66">
         <v>3562.5</v>
       </c>
-      <c r="M66">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="AI66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2353,19 +3094,31 @@
         <v>5</v>
       </c>
       <c r="J67">
+        <v>786</v>
+      </c>
+      <c r="R67">
+        <v>-786</v>
+      </c>
+      <c r="AD67">
+        <v>-786</v>
+      </c>
+      <c r="AE67">
         <v>396.9</v>
       </c>
-      <c r="K67">
+      <c r="AF67">
         <v>8335</v>
       </c>
-      <c r="L67">
+      <c r="AG67">
+        <v>9121</v>
+      </c>
+      <c r="AH67">
         <v>7938.1</v>
       </c>
-      <c r="M67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="AI67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2382,19 +3135,25 @@
         <v>12</v>
       </c>
       <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="AE68">
         <v>310.61</v>
       </c>
-      <c r="K68">
+      <c r="AF68">
         <v>2899</v>
       </c>
-      <c r="L68">
+      <c r="AG68">
+        <v>2899</v>
+      </c>
+      <c r="AH68">
         <v>2588.39</v>
       </c>
-      <c r="M68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="AI68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2411,19 +3170,25 @@
         <v>12</v>
       </c>
       <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="AE69">
         <v>160.18</v>
       </c>
-      <c r="K69">
+      <c r="AF69">
         <v>1495</v>
       </c>
-      <c r="L69">
+      <c r="AG69">
+        <v>1495</v>
+      </c>
+      <c r="AH69">
         <v>1334.82</v>
       </c>
-      <c r="M69">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="AI69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2440,19 +3205,25 @@
         <v>12</v>
       </c>
       <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="AE70">
         <v>160.18</v>
       </c>
-      <c r="K70">
+      <c r="AF70">
         <v>1495</v>
       </c>
-      <c r="L70">
+      <c r="AG70">
+        <v>1495</v>
+      </c>
+      <c r="AH70">
         <v>1334.82</v>
       </c>
-      <c r="M70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="AI70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2469,42 +3240,60 @@
         <v>5</v>
       </c>
       <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="AE71">
         <v>49.76</v>
       </c>
-      <c r="K71">
+      <c r="AF71">
         <v>1045</v>
       </c>
-      <c r="L71">
+      <c r="AG71">
+        <v>1045</v>
+      </c>
+      <c r="AH71">
         <v>995.24</v>
       </c>
-      <c r="M71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="AI71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
+      <c r="C72">
+        <v>2340</v>
+      </c>
+      <c r="H72">
+        <v>2340</v>
+      </c>
       <c r="I72">
         <v>12</v>
       </c>
       <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="AE72">
         <v>138.75</v>
       </c>
-      <c r="K72">
+      <c r="AF72">
         <v>1295</v>
       </c>
-      <c r="L72">
+      <c r="AG72">
+        <v>1295</v>
+      </c>
+      <c r="AH72">
         <v>1156.25</v>
       </c>
-      <c r="M72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="AI72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2524,19 +3313,31 @@
         <v>12</v>
       </c>
       <c r="J73">
+        <v>163</v>
+      </c>
+      <c r="U73">
+        <v>-163</v>
+      </c>
+      <c r="AC73">
+        <v>-163</v>
+      </c>
+      <c r="AE73">
         <v>614.36</v>
       </c>
-      <c r="K73">
+      <c r="AF73">
         <v>5734</v>
       </c>
-      <c r="L73">
+      <c r="AG73">
+        <v>5897</v>
+      </c>
+      <c r="AH73">
         <v>5119.64</v>
       </c>
-      <c r="M73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="AI73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2553,42 +3354,60 @@
         <v>5</v>
       </c>
       <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="AE74">
         <v>28.1</v>
       </c>
-      <c r="K74">
+      <c r="AF74">
         <v>590</v>
       </c>
-      <c r="L74">
+      <c r="AG74">
+        <v>590</v>
+      </c>
+      <c r="AH74">
         <v>561.9</v>
       </c>
-      <c r="M74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="AI74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
+      <c r="C75">
+        <v>4080</v>
+      </c>
+      <c r="H75">
+        <v>4080</v>
+      </c>
       <c r="I75">
         <v>12</v>
       </c>
       <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="AE75">
         <v>373.93</v>
       </c>
-      <c r="K75">
+      <c r="AF75">
         <v>3490</v>
       </c>
-      <c r="L75">
+      <c r="AG75">
+        <v>3490</v>
+      </c>
+      <c r="AH75">
         <v>3116.07</v>
       </c>
-      <c r="M75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="AI75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2605,19 +3424,25 @@
         <v>12</v>
       </c>
       <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="AE76">
         <v>669.21</v>
       </c>
-      <c r="K76">
+      <c r="AF76">
         <v>6246</v>
       </c>
-      <c r="L76">
+      <c r="AG76">
+        <v>6246</v>
+      </c>
+      <c r="AH76">
         <v>5576.79</v>
       </c>
-      <c r="M76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="AI76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2634,19 +3459,25 @@
         <v>12</v>
       </c>
       <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="AE77">
         <v>705.86</v>
       </c>
-      <c r="K77">
+      <c r="AF77">
         <v>6588</v>
       </c>
-      <c r="L77">
+      <c r="AG77">
+        <v>6588</v>
+      </c>
+      <c r="AH77">
         <v>5882.14</v>
       </c>
-      <c r="M77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="AI77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2666,42 +3497,75 @@
         <v>5</v>
       </c>
       <c r="J78">
+        <v>83</v>
+      </c>
+      <c r="R78">
+        <v>-32.85</v>
+      </c>
+      <c r="AD78">
+        <v>-32.85</v>
+      </c>
+      <c r="AE78">
         <v>48.2</v>
       </c>
-      <c r="K78">
+      <c r="AF78">
         <v>1012.15</v>
       </c>
-      <c r="L78">
+      <c r="AG78">
+        <v>1045</v>
+      </c>
+      <c r="AH78">
         <v>963.9499999999999</v>
       </c>
-      <c r="M78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="AI78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
+      <c r="C79">
+        <v>2640</v>
+      </c>
+      <c r="G79">
+        <v>-83</v>
+      </c>
+      <c r="H79">
+        <v>2557</v>
+      </c>
       <c r="I79">
         <v>12</v>
       </c>
       <c r="J79">
+        <v>83</v>
+      </c>
+      <c r="V79">
+        <v>-50.15</v>
+      </c>
+      <c r="AD79">
+        <v>-50.15</v>
+      </c>
+      <c r="AE79">
         <v>165.52</v>
       </c>
-      <c r="K79">
+      <c r="AF79">
         <v>1544.85</v>
       </c>
-      <c r="L79">
+      <c r="AG79">
+        <v>1595</v>
+      </c>
+      <c r="AH79">
         <v>1379.33</v>
       </c>
-      <c r="M79">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="AI79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2718,19 +3582,25 @@
         <v>12</v>
       </c>
       <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="AE80">
         <v>604.61</v>
       </c>
-      <c r="K80">
+      <c r="AF80">
         <v>5643</v>
       </c>
-      <c r="L80">
+      <c r="AG80">
+        <v>5643</v>
+      </c>
+      <c r="AH80">
         <v>5038.39</v>
       </c>
-      <c r="M80">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="AI80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2747,19 +3617,25 @@
         <v>12</v>
       </c>
       <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="AE81">
         <v>149.46</v>
       </c>
-      <c r="K81">
+      <c r="AF81">
         <v>1395</v>
       </c>
-      <c r="L81">
+      <c r="AG81">
+        <v>1395</v>
+      </c>
+      <c r="AH81">
         <v>1245.54</v>
       </c>
-      <c r="M81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="AI81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2779,19 +3655,31 @@
         <v>12</v>
       </c>
       <c r="J82">
+        <v>207</v>
+      </c>
+      <c r="V82">
+        <v>-207</v>
+      </c>
+      <c r="AD82">
+        <v>-207</v>
+      </c>
+      <c r="AE82">
         <v>319.61</v>
       </c>
-      <c r="K82">
+      <c r="AF82">
         <v>2983</v>
       </c>
-      <c r="L82">
+      <c r="AG82">
+        <v>3190</v>
+      </c>
+      <c r="AH82">
         <v>2663.39</v>
       </c>
-      <c r="M82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="AI82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2808,19 +3696,25 @@
         <v>12</v>
       </c>
       <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="AE83">
         <v>395.36</v>
       </c>
-      <c r="K83">
+      <c r="AF83">
         <v>3690</v>
       </c>
-      <c r="L83">
+      <c r="AG83">
+        <v>3690</v>
+      </c>
+      <c r="AH83">
         <v>3294.64</v>
       </c>
-      <c r="M83">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="AI83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2837,19 +3731,25 @@
         <v>5</v>
       </c>
       <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="AE84">
         <v>16.62</v>
       </c>
-      <c r="K84">
+      <c r="AF84">
         <v>349</v>
       </c>
-      <c r="L84">
+      <c r="AG84">
+        <v>349</v>
+      </c>
+      <c r="AH84">
         <v>332.38</v>
       </c>
-      <c r="M84">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="AI84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2869,65 +3769,119 @@
         <v>5</v>
       </c>
       <c r="J85">
+        <v>358</v>
+      </c>
+      <c r="R85">
+        <v>-24.51</v>
+      </c>
+      <c r="AD85">
+        <v>-24.51</v>
+      </c>
+      <c r="AE85">
         <v>95.02</v>
       </c>
-      <c r="K85">
+      <c r="AF85">
         <v>1995.49</v>
       </c>
-      <c r="L85">
+      <c r="AG85">
+        <v>2020</v>
+      </c>
+      <c r="AH85">
         <v>1900.47</v>
       </c>
-      <c r="M85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="AI85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86">
         <v>4</v>
       </c>
+      <c r="C86">
+        <v>29506</v>
+      </c>
+      <c r="G86">
+        <v>-358</v>
+      </c>
+      <c r="H86">
+        <v>29148</v>
+      </c>
       <c r="I86">
         <v>12</v>
       </c>
       <c r="J86">
+        <v>358</v>
+      </c>
+      <c r="V86">
+        <v>-311.68</v>
+      </c>
+      <c r="AD86">
+        <v>-311.68</v>
+      </c>
+      <c r="AE86">
         <v>2718.89</v>
       </c>
-      <c r="K86">
+      <c r="AF86">
         <v>25376.33</v>
       </c>
-      <c r="L86">
+      <c r="AG86">
+        <v>25688.01</v>
+      </c>
+      <c r="AH86">
         <v>22657.44</v>
       </c>
-      <c r="M86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="AI86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
+      <c r="C87">
+        <v>29506</v>
+      </c>
+      <c r="G87">
+        <v>-358</v>
+      </c>
+      <c r="H87">
+        <v>29148</v>
+      </c>
       <c r="I87">
         <v>18</v>
       </c>
       <c r="J87">
+        <v>358</v>
+      </c>
+      <c r="Z87">
+        <v>-21.82</v>
+      </c>
+      <c r="AD87">
+        <v>-21.82</v>
+      </c>
+      <c r="AE87">
         <v>270.94</v>
       </c>
-      <c r="K87">
+      <c r="AF87">
         <v>1776.18</v>
       </c>
-      <c r="L87">
+      <c r="AG87">
+        <v>1798</v>
+      </c>
+      <c r="AH87">
         <v>1505.24</v>
       </c>
-      <c r="M87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="AI87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2944,19 +3898,25 @@
         <v>12</v>
       </c>
       <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="AE88">
         <v>513.11</v>
       </c>
-      <c r="K88">
+      <c r="AF88">
         <v>4789</v>
       </c>
-      <c r="L88">
+      <c r="AG88">
+        <v>4789</v>
+      </c>
+      <c r="AH88">
         <v>4275.89</v>
       </c>
-      <c r="M88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="AI88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2973,42 +3933,60 @@
         <v>5</v>
       </c>
       <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="AE89">
         <v>47.38</v>
       </c>
-      <c r="K89">
+      <c r="AF89">
         <v>995</v>
       </c>
-      <c r="L89">
+      <c r="AG89">
+        <v>995</v>
+      </c>
+      <c r="AH89">
         <v>947.62</v>
       </c>
-      <c r="M89">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="AI89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90">
         <v>6</v>
       </c>
+      <c r="C90">
+        <v>11765</v>
+      </c>
+      <c r="H90">
+        <v>11765</v>
+      </c>
       <c r="I90">
         <v>12</v>
       </c>
       <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="AE90">
         <v>1153.93</v>
       </c>
-      <c r="K90">
+      <c r="AF90">
         <v>10770</v>
       </c>
-      <c r="L90">
+      <c r="AG90">
+        <v>10770</v>
+      </c>
+      <c r="AH90">
         <v>9616.07</v>
       </c>
-      <c r="M90">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="AI90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3028,19 +4006,31 @@
         <v>5</v>
       </c>
       <c r="J91">
+        <v>487</v>
+      </c>
+      <c r="R91">
+        <v>-487</v>
+      </c>
+      <c r="AD91">
+        <v>-487</v>
+      </c>
+      <c r="AE91">
         <v>38.48</v>
       </c>
-      <c r="K91">
+      <c r="AF91">
         <v>808</v>
       </c>
-      <c r="L91">
+      <c r="AG91">
+        <v>1295</v>
+      </c>
+      <c r="AH91">
         <v>769.52</v>
       </c>
-      <c r="M91">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="AI91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3060,19 +4050,31 @@
         <v>5</v>
       </c>
       <c r="J92">
+        <v>2000</v>
+      </c>
+      <c r="R92">
+        <v>-2000</v>
+      </c>
+      <c r="AD92">
+        <v>-2000</v>
+      </c>
+      <c r="AE92">
         <v>62.33</v>
       </c>
-      <c r="K92">
+      <c r="AF92">
         <v>1309</v>
       </c>
-      <c r="L92">
+      <c r="AG92">
+        <v>3309</v>
+      </c>
+      <c r="AH92">
         <v>1246.67</v>
       </c>
-      <c r="M92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="AI92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3092,19 +4094,31 @@
         <v>5</v>
       </c>
       <c r="J93">
+        <v>539</v>
+      </c>
+      <c r="R93">
+        <v>-539</v>
+      </c>
+      <c r="AD93">
+        <v>-539</v>
+      </c>
+      <c r="AE93">
         <v>21.95</v>
       </c>
-      <c r="K93">
+      <c r="AF93">
         <v>461</v>
       </c>
-      <c r="L93">
+      <c r="AG93">
+        <v>1000</v>
+      </c>
+      <c r="AH93">
         <v>439.05</v>
       </c>
-      <c r="M93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="AI93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3121,42 +4135,60 @@
         <v>5</v>
       </c>
       <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="AE94">
         <v>25.95</v>
       </c>
-      <c r="K94">
+      <c r="AF94">
         <v>545</v>
       </c>
-      <c r="L94">
+      <c r="AG94">
+        <v>545</v>
+      </c>
+      <c r="AH94">
         <v>519.05</v>
       </c>
-      <c r="M94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="AI94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
+      <c r="C95">
+        <v>1790</v>
+      </c>
+      <c r="H95">
+        <v>1790</v>
+      </c>
       <c r="I95">
         <v>12</v>
       </c>
       <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="AE95">
         <v>133.39</v>
       </c>
-      <c r="K95">
+      <c r="AF95">
         <v>1245</v>
       </c>
-      <c r="L95">
+      <c r="AG95">
+        <v>1245</v>
+      </c>
+      <c r="AH95">
         <v>1111.61</v>
       </c>
-      <c r="M95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="AI95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3173,19 +4205,25 @@
         <v>5</v>
       </c>
       <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="AE96">
         <v>47.62</v>
       </c>
-      <c r="K96">
+      <c r="AF96">
         <v>1000</v>
       </c>
-      <c r="L96">
+      <c r="AG96">
+        <v>1000</v>
+      </c>
+      <c r="AH96">
         <v>952.38</v>
       </c>
-      <c r="M96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="AI96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3202,19 +4240,25 @@
         <v>5</v>
       </c>
       <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="AE97">
         <v>47.62</v>
       </c>
-      <c r="K97">
+      <c r="AF97">
         <v>1000</v>
       </c>
-      <c r="L97">
+      <c r="AG97">
+        <v>1000</v>
+      </c>
+      <c r="AH97">
         <v>952.38</v>
       </c>
-      <c r="M97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="AI97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3231,15 +4275,21 @@
         <v>5</v>
       </c>
       <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="AE98">
         <v>47.62</v>
       </c>
-      <c r="K98">
+      <c r="AF98">
         <v>1000</v>
       </c>
-      <c r="L98">
+      <c r="AG98">
+        <v>1000</v>
+      </c>
+      <c r="AH98">
         <v>952.38</v>
       </c>
-      <c r="M98">
+      <c r="AI98">
         <v>1</v>
       </c>
     </row>

</xml_diff>